<commit_message>
Location Update Multiple Users Same Device ( currently double the work).
</commit_message>
<xml_diff>
--- a/NeverEatAlone/NEA_Issues.xlsx
+++ b/NeverEatAlone/NEA_Issues.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="28">
   <si>
     <t>ISSUE</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Profile Updates</t>
   </si>
   <si>
-    <t>Nearby List</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -100,6 +97,12 @@
   </si>
   <si>
     <t>Firebase integration</t>
+  </si>
+  <si>
+    <t>Mutliple Users same device Location Persistence</t>
+  </si>
+  <si>
+    <t>Nearby Contacts List</t>
   </si>
 </sst>
 </file>
@@ -549,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A14"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -658,13 +661,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -678,9 +681,11 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
@@ -713,7 +718,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
@@ -731,14 +736,14 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -749,14 +754,14 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -767,7 +772,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>4</v>
@@ -787,7 +792,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>4</v>
@@ -807,7 +812,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>4</v>
@@ -827,14 +832,14 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -845,7 +850,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>4</v>
@@ -865,7 +870,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>4</v>
@@ -885,14 +890,14 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -901,56 +906,40 @@
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="68">
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
+  <mergeCells count="72">
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="C27:C28"/>
@@ -963,14 +952,54 @@
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>